<commit_message>
updated dir and naming conventions
</commit_message>
<xml_diff>
--- a/NETN_water_summaries_metadata.xlsx
+++ b/NETN_water_summaries_metadata.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Diana\Documents\NETN\Water\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\NETN\R_Dev\Water\NETN_water_summaries\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05E66980-BD25-4E64-A4F7-66AE15B74001}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330"/>
+    <workbookView xWindow="4080" yWindow="3285" windowWidth="21600" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="48">
   <si>
     <t>File name</t>
   </si>
@@ -45,9 +46,6 @@
     <t>./rmd/</t>
   </si>
   <si>
-    <t>./scripts/</t>
-  </si>
-  <si>
     <t>./</t>
   </si>
   <si>
@@ -66,9 +64,6 @@
     <t>header_manual</t>
   </si>
   <si>
-    <t>generate_briefs_all_parks</t>
-  </si>
-  <si>
     <t>boundboxes</t>
   </si>
   <si>
@@ -172,12 +167,15 @@
   </si>
   <si>
     <t>ACAD_automated_summary</t>
+  </si>
+  <si>
+    <t>generate_summaries_all_parks</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -500,11 +498,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -517,7 +515,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>4</v>
@@ -537,10 +535,10 @@
         <v>5</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="60" x14ac:dyDescent="0.25">
@@ -551,10 +549,10 @@
         <v>5</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="105" x14ac:dyDescent="0.25">
@@ -565,10 +563,10 @@
         <v>5</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="60" x14ac:dyDescent="0.25">
@@ -579,10 +577,10 @@
         <v>5</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="60" x14ac:dyDescent="0.25">
@@ -593,122 +591,122 @@
         <v>5</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="2" t="s">
-        <v>17</v>
-      </c>
       <c r="D7" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="75" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>13</v>
+        <v>47</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="105" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="90" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="2" t="s">
-        <v>8</v>
-      </c>
       <c r="D11" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D12" s="1" t="s">
         <v>28</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="75" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="75" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B14" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D14" s="3" t="s">
         <v>38</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -718,7 +716,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B2:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -733,27 +731,27 @@
   <sheetData>
     <row r="2" spans="2:2" ht="30" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="2:2" ht="45" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="2:2" ht="30" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="2:2" ht="45" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="6" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>